<commit_message>
Refactor utility rendering logic to handle errors and improve readability
</commit_message>
<xml_diff>
--- a/Utenze.xlsx
+++ b/Utenze.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Cabinet</t>
   </si>
@@ -23,9 +23,6 @@
   </si>
   <si>
     <t>Utenza</t>
-  </si>
-  <si>
-    <t>Cab1 Generale1</t>
   </si>
   <si>
     <t>Cab2 Generale1</t>
@@ -39,7 +36,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,12 +47,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -87,19 +78,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -409,15 +394,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="7.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="16.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="7.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="16.862142857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -431,37 +416,26 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>